<commit_message>
Use Home Page - Side Drop panel
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/assets/excel/drop down menu-navigator.xlsx
+++ b/assets/excel/drop down menu-navigator.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Business</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,10 +35,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Product</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Technical support</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -67,10 +63,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Web Software I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>K-COL Design (SRC)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -99,30 +91,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DataBase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>KS-Code</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>현대제철 H형강</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POS H형강</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Web Software II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Soil Protection</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Slim Box - MTL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -139,10 +111,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ex-Slim-Beam  Production Managemet System</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DMIS for K-COL Project</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -176,6 +144,46 @@
   </si>
   <si>
     <t xml:space="preserve">EX-Slim-Beam </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Soil Protection CIP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXTRA Slim-Beam  Production Managemet System</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WebSoftware I
+     K-COL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WebSoftware II
+    Composite Beam</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">WebSoftware III
+   EXTRA Slim Beam </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WebSoftware IV
+   Column</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product Schedule</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXTRA Slim-Beam</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Non_Composie_CastellatedBeam_Design_Calculatoor.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -222,9 +230,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -869,10 +880,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E4:F44"/>
+  <dimension ref="E4:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -888,175 +899,190 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F5" t="s">
+    <row r="10" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F9" t="s">
-        <v>31</v>
+      <c r="F10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="5:6" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="5:6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="5:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="E14" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="5:6" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E17" t="s">
-        <v>22</v>
-      </c>
+    <row r="17" spans="5:13" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="5:13" ht="33" x14ac:dyDescent="0.3">
+      <c r="E20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F18" t="s">
+      <c r="M21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="5:13" ht="33" x14ac:dyDescent="0.3">
+      <c r="E23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F19" t="s">
+    <row r="25" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="5:13" ht="33" x14ac:dyDescent="0.3">
+      <c r="E27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F24" t="s">
+    <row r="28" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E26" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E29" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F30" t="s">
+    <row r="32" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>36</v>
+      </c>
+      <c r="F38" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F31" t="s">
+    <row r="39" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E33" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E36" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F38" t="s">
+    <row r="40" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E40" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="42" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E42" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="F42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E44" t="s">
-        <v>33</v>
+      <c r="F44" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E50" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>